<commit_message>
- took over the updated recode function for smoking status from LISA
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{85C256F3-5FC3-41A9-9720-7A0E43545612}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF5B1BC-B852-45B4-AC2E-96FD6C5B0F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,10 +481,6 @@
     <t>Intake of cheese curd, quark and cottage [g/d]</t>
   </si>
   <si>
-    <t xml:space="preserve">FFQQUARK_15
-</t>
-  </si>
-  <si>
     <t>CHEESE_0505</t>
   </si>
   <si>
@@ -1408,6 +1404,9 @@
   </si>
   <si>
     <t>compatible, because it is integer and we want decimal</t>
+  </si>
+  <si>
+    <t>FFQQUARK_15</t>
   </si>
 </sst>
 </file>
@@ -2380,9 +2379,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B129" sqref="B129:K129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,7 +2523,7 @@
         <v>21</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>16</v>
@@ -3490,7 +3489,7 @@
         <v>14</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>126</v>
+        <v>389</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>21</v>
@@ -3510,25 +3509,25 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="D35" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="D35" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1" t="s">
@@ -3543,19 +3542,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="D36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>21</v>
@@ -3576,19 +3575,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="D37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="D37" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>21</v>
@@ -3609,11 +3608,11 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C38" s="21" t="s">
-        <v>138</v>
-      </c>
       <c r="D38" t="s">
         <v>24</v>
       </c>
@@ -3621,7 +3620,7 @@
         <v>14</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>21</v>
@@ -3642,10 +3641,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="D39" t="s">
         <v>24</v>
@@ -3674,10 +3673,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>141</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>142</v>
       </c>
       <c r="D40" t="s">
         <v>24</v>
@@ -3706,25 +3705,25 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="D41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="D41" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>16</v>
@@ -3738,10 +3737,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" s="21" t="s">
         <v>147</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>148</v>
       </c>
       <c r="D42" t="s">
         <v>24</v>
@@ -3770,25 +3769,25 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="D43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>16</v>
@@ -3802,28 +3801,28 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="D44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="D44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H44" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="I44" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="I44" s="7" t="s">
-        <v>157</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>33</v>
@@ -3837,11 +3836,11 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C45" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>159</v>
-      </c>
       <c r="D45" t="s">
         <v>24</v>
       </c>
@@ -3849,13 +3848,13 @@
         <v>14</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>16</v>
@@ -3869,10 +3868,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="21" t="s">
         <v>160</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>161</v>
       </c>
       <c r="D46" t="s">
         <v>24</v>
@@ -3901,25 +3900,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C47" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="D47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>163</v>
-      </c>
-      <c r="D47" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>16</v>
@@ -3933,10 +3932,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="21" t="s">
         <v>166</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>167</v>
       </c>
       <c r="D48" t="s">
         <v>24</v>
@@ -3965,19 +3964,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="D49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="D49" t="s">
-        <v>24</v>
-      </c>
-      <c r="E49" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>21</v>
@@ -3997,11 +3996,11 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C50" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>172</v>
-      </c>
       <c r="D50" t="s">
         <v>24</v>
       </c>
@@ -4009,7 +4008,7 @@
         <v>14</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G50" s="25" t="s">
         <v>21</v>
@@ -4030,11 +4029,11 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="C51" s="21" t="s">
-        <v>174</v>
-      </c>
       <c r="D51" t="s">
         <v>24</v>
       </c>
@@ -4042,13 +4041,13 @@
         <v>14</v>
       </c>
       <c r="F51" s="26" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G51" s="25" t="s">
         <v>54</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="25" t="s">
@@ -4063,28 +4062,28 @@
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="C52" s="21" t="s">
+      <c r="D52" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="D52" t="s">
-        <v>24</v>
-      </c>
-      <c r="E52" t="s">
-        <v>14</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H52" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="I52" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>33</v>
@@ -4098,11 +4097,11 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="C53" s="21" t="s">
-        <v>182</v>
-      </c>
       <c r="D53" t="s">
         <v>24</v>
       </c>
@@ -4110,16 +4109,16 @@
         <v>14</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H53" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="I53" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>33</v>
@@ -4133,19 +4132,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="D54" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="D54" t="s">
-        <v>24</v>
-      </c>
-      <c r="E54" t="s">
-        <v>14</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>21</v>
@@ -4165,10 +4164,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="21" t="s">
         <v>186</v>
-      </c>
-      <c r="C55" s="21" t="s">
-        <v>187</v>
       </c>
       <c r="D55" t="s">
         <v>24</v>
@@ -4197,10 +4196,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C56" s="21" t="s">
         <v>188</v>
-      </c>
-      <c r="C56" s="21" t="s">
-        <v>189</v>
       </c>
       <c r="D56" t="s">
         <v>24</v>
@@ -4229,10 +4228,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C57" s="21" t="s">
         <v>190</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>191</v>
       </c>
       <c r="D57" t="s">
         <v>24</v>
@@ -4261,19 +4260,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C58" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="D58" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="D58" t="s">
-        <v>24</v>
-      </c>
-      <c r="E58" t="s">
-        <v>14</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>194</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>21</v>
@@ -4293,10 +4292,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C59" s="21" t="s">
         <v>195</v>
-      </c>
-      <c r="C59" s="21" t="s">
-        <v>196</v>
       </c>
       <c r="D59" t="s">
         <v>24</v>
@@ -4325,10 +4324,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C60" s="21" t="s">
         <v>197</v>
-      </c>
-      <c r="C60" s="21" t="s">
-        <v>198</v>
       </c>
       <c r="D60" t="s">
         <v>24</v>
@@ -4357,10 +4356,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C61" s="21" t="s">
         <v>199</v>
-      </c>
-      <c r="C61" s="21" t="s">
-        <v>200</v>
       </c>
       <c r="D61" t="s">
         <v>24</v>
@@ -4389,10 +4388,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C62" s="21" t="s">
         <v>201</v>
-      </c>
-      <c r="C62" s="21" t="s">
-        <v>202</v>
       </c>
       <c r="D62" t="s">
         <v>24</v>
@@ -4421,10 +4420,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C63" s="21" t="s">
         <v>203</v>
-      </c>
-      <c r="C63" s="21" t="s">
-        <v>204</v>
       </c>
       <c r="D63" t="s">
         <v>24</v>
@@ -4453,10 +4452,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C64" s="21" t="s">
         <v>205</v>
-      </c>
-      <c r="C64" s="21" t="s">
-        <v>206</v>
       </c>
       <c r="D64" t="s">
         <v>24</v>
@@ -4485,10 +4484,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C65" s="21" t="s">
         <v>207</v>
-      </c>
-      <c r="C65" s="21" t="s">
-        <v>208</v>
       </c>
       <c r="D65" t="s">
         <v>24</v>
@@ -4517,25 +4516,25 @@
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="C66" s="21" t="s">
+      <c r="D66" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="D66" t="s">
-        <v>24</v>
-      </c>
-      <c r="E66" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>16</v>
@@ -4549,19 +4548,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C67" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="C67" s="21" t="s">
+      <c r="D67" t="s">
+        <v>24</v>
+      </c>
+      <c r="E67" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="D67" t="s">
-        <v>24</v>
-      </c>
-      <c r="E67" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>21</v>
@@ -4581,25 +4580,25 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C68" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="C68" s="21" t="s">
+      <c r="D68" t="s">
+        <v>24</v>
+      </c>
+      <c r="E68" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="D68" t="s">
-        <v>24</v>
-      </c>
-      <c r="E68" t="s">
-        <v>14</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>16</v>
@@ -4613,25 +4612,25 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C69" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="C69" s="21" t="s">
+      <c r="D69" t="s">
+        <v>24</v>
+      </c>
+      <c r="E69" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="D69" t="s">
-        <v>24</v>
-      </c>
-      <c r="E69" t="s">
-        <v>14</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>16</v>
@@ -4645,10 +4644,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C70" s="21" t="s">
         <v>224</v>
-      </c>
-      <c r="C70" s="21" t="s">
-        <v>225</v>
       </c>
       <c r="D70" t="s">
         <v>24</v>
@@ -4677,25 +4676,25 @@
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C71" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="C71" s="21" t="s">
+      <c r="D71" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="7" t="s">
         <v>227</v>
-      </c>
-      <c r="D71" t="s">
-        <v>24</v>
-      </c>
-      <c r="E71" t="s">
-        <v>14</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>228</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>16</v>
@@ -4709,19 +4708,19 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>229</v>
+      </c>
+      <c r="C72" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="D72" t="s">
+        <v>24</v>
+      </c>
+      <c r="E72" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="D72" t="s">
-        <v>24</v>
-      </c>
-      <c r="E72" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>21</v>
@@ -4742,10 +4741,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>232</v>
+      </c>
+      <c r="C73" s="21" t="s">
         <v>233</v>
-      </c>
-      <c r="C73" s="21" t="s">
-        <v>234</v>
       </c>
       <c r="D73" t="s">
         <v>24</v>
@@ -4774,25 +4773,25 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>234</v>
+      </c>
+      <c r="C74" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="C74" s="21" t="s">
+      <c r="D74" t="s">
+        <v>24</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="D74" t="s">
-        <v>24</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>237</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>16</v>
@@ -4806,25 +4805,25 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>238</v>
+      </c>
+      <c r="C75" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="C75" s="21" t="s">
+      <c r="D75" t="s">
+        <v>24</v>
+      </c>
+      <c r="E75" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="D75" t="s">
-        <v>24</v>
-      </c>
-      <c r="E75" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>16</v>
@@ -4838,25 +4837,25 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
+        <v>242</v>
+      </c>
+      <c r="C76" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="C76" s="21" t="s">
+      <c r="D76" t="s">
+        <v>24</v>
+      </c>
+      <c r="E76" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="D76" t="s">
-        <v>24</v>
-      </c>
-      <c r="E76" t="s">
-        <v>14</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>16</v>
@@ -4870,25 +4869,25 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>246</v>
+      </c>
+      <c r="C77" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="C77" s="21" t="s">
+      <c r="D77" t="s">
+        <v>24</v>
+      </c>
+      <c r="E77" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="D77" t="s">
-        <v>24</v>
-      </c>
-      <c r="E77" t="s">
-        <v>14</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>16</v>
@@ -4902,10 +4901,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>250</v>
+      </c>
+      <c r="C78" s="21" t="s">
         <v>251</v>
-      </c>
-      <c r="C78" s="21" t="s">
-        <v>252</v>
       </c>
       <c r="D78" t="s">
         <v>24</v>
@@ -4934,10 +4933,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>252</v>
+      </c>
+      <c r="C79" s="21" t="s">
         <v>253</v>
-      </c>
-      <c r="C79" s="21" t="s">
-        <v>254</v>
       </c>
       <c r="D79" t="s">
         <v>24</v>
@@ -4966,10 +4965,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>254</v>
+      </c>
+      <c r="C80" s="21" t="s">
         <v>255</v>
-      </c>
-      <c r="C80" s="21" t="s">
-        <v>256</v>
       </c>
       <c r="D80" t="s">
         <v>24</v>
@@ -4998,25 +4997,25 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>256</v>
+      </c>
+      <c r="C81" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="C81" s="21" t="s">
+      <c r="D81" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="D81" t="s">
-        <v>24</v>
-      </c>
-      <c r="E81" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>16</v>
@@ -5030,10 +5029,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>260</v>
+      </c>
+      <c r="C82" s="21" t="s">
         <v>261</v>
-      </c>
-      <c r="C82" s="21" t="s">
-        <v>262</v>
       </c>
       <c r="D82" t="s">
         <v>24</v>
@@ -5062,25 +5061,25 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>262</v>
+      </c>
+      <c r="C83" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="C83" s="21" t="s">
+      <c r="D83" t="s">
+        <v>24</v>
+      </c>
+      <c r="E83" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="D83" t="s">
-        <v>24</v>
-      </c>
-      <c r="E83" t="s">
-        <v>14</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>265</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J83" s="1" t="s">
         <v>16</v>
@@ -5094,19 +5093,19 @@
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C84" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="C84" s="21" t="s">
+      <c r="D84" t="s">
+        <v>24</v>
+      </c>
+      <c r="E84" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="D84" t="s">
-        <v>24</v>
-      </c>
-      <c r="E84" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>269</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>21</v>
@@ -5126,19 +5125,19 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
+        <v>269</v>
+      </c>
+      <c r="C85" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="C85" s="21" t="s">
+      <c r="D85" t="s">
+        <v>24</v>
+      </c>
+      <c r="E85" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="4" t="s">
         <v>271</v>
-      </c>
-      <c r="D85" t="s">
-        <v>24</v>
-      </c>
-      <c r="E85" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>272</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>21</v>
@@ -5158,19 +5157,19 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
+        <v>272</v>
+      </c>
+      <c r="C86" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="C86" s="21" t="s">
+      <c r="D86" t="s">
+        <v>24</v>
+      </c>
+      <c r="E86" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="D86" t="s">
-        <v>24</v>
-      </c>
-      <c r="E86" t="s">
-        <v>14</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>275</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>21</v>
@@ -5191,10 +5190,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
+        <v>275</v>
+      </c>
+      <c r="C87" s="21" t="s">
         <v>276</v>
-      </c>
-      <c r="C87" s="21" t="s">
-        <v>277</v>
       </c>
       <c r="D87" t="s">
         <v>24</v>
@@ -5223,10 +5222,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
+        <v>277</v>
+      </c>
+      <c r="C88" s="21" t="s">
         <v>278</v>
-      </c>
-      <c r="C88" s="21" t="s">
-        <v>279</v>
       </c>
       <c r="D88" t="s">
         <v>24</v>
@@ -5255,10 +5254,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
+        <v>279</v>
+      </c>
+      <c r="C89" s="21" t="s">
         <v>280</v>
-      </c>
-      <c r="C89" s="21" t="s">
-        <v>281</v>
       </c>
       <c r="D89" t="s">
         <v>24</v>
@@ -5287,25 +5286,25 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
+        <v>281</v>
+      </c>
+      <c r="C90" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="C90" s="21" t="s">
+      <c r="D90" t="s">
+        <v>24</v>
+      </c>
+      <c r="E90" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="D90" t="s">
-        <v>24</v>
-      </c>
-      <c r="E90" t="s">
-        <v>14</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>16</v>
@@ -5319,25 +5318,25 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
+        <v>285</v>
+      </c>
+      <c r="C91" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="C91" s="21" t="s">
+      <c r="D91" t="s">
+        <v>24</v>
+      </c>
+      <c r="E91" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="D91" t="s">
-        <v>24</v>
-      </c>
-      <c r="E91" t="s">
-        <v>14</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>288</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J91" s="1" t="s">
         <v>16</v>
@@ -5351,19 +5350,19 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
+        <v>289</v>
+      </c>
+      <c r="C92" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="C92" s="21" t="s">
+      <c r="D92" t="s">
+        <v>24</v>
+      </c>
+      <c r="E92" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="4" t="s">
         <v>291</v>
-      </c>
-      <c r="D92" t="s">
-        <v>24</v>
-      </c>
-      <c r="E92" t="s">
-        <v>14</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>292</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>21</v>
@@ -5383,25 +5382,25 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
+        <v>292</v>
+      </c>
+      <c r="C93" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="C93" s="21" t="s">
+      <c r="D93" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" t="s">
+        <v>14</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="D93" t="s">
-        <v>24</v>
-      </c>
-      <c r="E93" t="s">
-        <v>14</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>295</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J93" s="1" t="s">
         <v>16</v>
@@ -5415,25 +5414,25 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
+        <v>296</v>
+      </c>
+      <c r="C94" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="C94" s="21" t="s">
+      <c r="D94" t="s">
+        <v>24</v>
+      </c>
+      <c r="E94" t="s">
+        <v>14</v>
+      </c>
+      <c r="F94" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="D94" t="s">
-        <v>24</v>
-      </c>
-      <c r="E94" t="s">
-        <v>14</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>16</v>
@@ -5447,25 +5446,25 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
+        <v>300</v>
+      </c>
+      <c r="C95" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="C95" s="21" t="s">
+      <c r="D95" t="s">
+        <v>24</v>
+      </c>
+      <c r="E95" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="D95" t="s">
-        <v>24</v>
-      </c>
-      <c r="E95" t="s">
-        <v>14</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>303</v>
       </c>
       <c r="G95" s="4" t="s">
         <v>54</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>16</v>
@@ -5479,19 +5478,19 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
+        <v>304</v>
+      </c>
+      <c r="C96" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="C96" s="21" t="s">
+      <c r="D96" t="s">
+        <v>24</v>
+      </c>
+      <c r="E96" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96" s="4" t="s">
         <v>306</v>
-      </c>
-      <c r="D96" t="s">
-        <v>24</v>
-      </c>
-      <c r="E96" t="s">
-        <v>14</v>
-      </c>
-      <c r="F96" s="4" t="s">
-        <v>307</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>21</v>
@@ -5500,13 +5499,13 @@
         <v>21</v>
       </c>
       <c r="I96" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J96" s="17" t="s">
         <v>33</v>
       </c>
       <c r="K96" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -5514,10 +5513,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
+        <v>309</v>
+      </c>
+      <c r="C97" s="21" t="s">
         <v>310</v>
-      </c>
-      <c r="C97" s="21" t="s">
-        <v>311</v>
       </c>
       <c r="D97" t="s">
         <v>24</v>
@@ -5546,11 +5545,11 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
+        <v>311</v>
+      </c>
+      <c r="C98" s="21" t="s">
         <v>312</v>
       </c>
-      <c r="C98" s="21" t="s">
-        <v>313</v>
-      </c>
       <c r="D98" t="s">
         <v>24</v>
       </c>
@@ -5558,7 +5557,7 @@
         <v>14</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>21</v>
@@ -5578,10 +5577,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
+        <v>313</v>
+      </c>
+      <c r="C99" s="21" t="s">
         <v>314</v>
-      </c>
-      <c r="C99" s="21" t="s">
-        <v>315</v>
       </c>
       <c r="D99" t="s">
         <v>24</v>
@@ -5610,10 +5609,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="C100" s="21" t="s">
         <v>316</v>
-      </c>
-      <c r="C100" s="21" t="s">
-        <v>317</v>
       </c>
       <c r="D100" t="s">
         <v>24</v>
@@ -5642,19 +5641,19 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>317</v>
+      </c>
+      <c r="C101" s="21" t="s">
         <v>318</v>
       </c>
-      <c r="C101" s="21" t="s">
+      <c r="D101" t="s">
+        <v>24</v>
+      </c>
+      <c r="E101" t="s">
+        <v>14</v>
+      </c>
+      <c r="F101" s="6" t="s">
         <v>319</v>
-      </c>
-      <c r="D101" t="s">
-        <v>24</v>
-      </c>
-      <c r="E101" t="s">
-        <v>14</v>
-      </c>
-      <c r="F101" s="6" t="s">
-        <v>320</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>21</v>
@@ -5674,19 +5673,19 @@
         <v>101</v>
       </c>
       <c r="B102" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="C102" s="23" t="s">
         <v>321</v>
       </c>
-      <c r="C102" s="23" t="s">
+      <c r="D102" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D102" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E102" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>323</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>21</v>
@@ -5707,19 +5706,19 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
+        <v>323</v>
+      </c>
+      <c r="C103" s="21" t="s">
         <v>324</v>
       </c>
-      <c r="C103" s="21" t="s">
+      <c r="D103" t="s">
+        <v>24</v>
+      </c>
+      <c r="E103" t="s">
+        <v>14</v>
+      </c>
+      <c r="F103" s="4" t="s">
         <v>325</v>
-      </c>
-      <c r="D103" t="s">
-        <v>24</v>
-      </c>
-      <c r="E103" t="s">
-        <v>14</v>
-      </c>
-      <c r="F103" s="4" t="s">
-        <v>326</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>21</v>
@@ -5739,10 +5738,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
+        <v>326</v>
+      </c>
+      <c r="C104" s="21" t="s">
         <v>327</v>
-      </c>
-      <c r="C104" s="21" t="s">
-        <v>328</v>
       </c>
       <c r="D104" t="s">
         <v>24</v>
@@ -5771,19 +5770,19 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
+        <v>328</v>
+      </c>
+      <c r="C105" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="C105" s="21" t="s">
+      <c r="D105" t="s">
+        <v>24</v>
+      </c>
+      <c r="E105" t="s">
+        <v>14</v>
+      </c>
+      <c r="F105" s="4" t="s">
         <v>330</v>
-      </c>
-      <c r="D105" t="s">
-        <v>24</v>
-      </c>
-      <c r="E105" t="s">
-        <v>14</v>
-      </c>
-      <c r="F105" s="4" t="s">
-        <v>331</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>21</v>
@@ -5803,10 +5802,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
+        <v>331</v>
+      </c>
+      <c r="C106" s="21" t="s">
         <v>332</v>
-      </c>
-      <c r="C106" s="21" t="s">
-        <v>333</v>
       </c>
       <c r="D106" t="s">
         <v>24</v>
@@ -5835,10 +5834,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
+        <v>333</v>
+      </c>
+      <c r="C107" s="21" t="s">
         <v>334</v>
-      </c>
-      <c r="C107" s="21" t="s">
-        <v>335</v>
       </c>
       <c r="D107" t="s">
         <v>24</v>
@@ -5867,19 +5866,19 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
+        <v>335</v>
+      </c>
+      <c r="C108" s="21" t="s">
         <v>336</v>
       </c>
-      <c r="C108" s="21" t="s">
+      <c r="D108" t="s">
+        <v>24</v>
+      </c>
+      <c r="E108" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="D108" t="s">
-        <v>24</v>
-      </c>
-      <c r="E108" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108" s="4" t="s">
-        <v>338</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>21</v>
@@ -5899,25 +5898,25 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>338</v>
+      </c>
+      <c r="C109" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="C109" s="21" t="s">
+      <c r="D109" t="s">
+        <v>24</v>
+      </c>
+      <c r="E109" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="D109" t="s">
-        <v>24</v>
-      </c>
-      <c r="E109" t="s">
-        <v>14</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>341</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J109" s="1" t="s">
         <v>16</v>
@@ -5931,10 +5930,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
+        <v>342</v>
+      </c>
+      <c r="C110" s="21" t="s">
         <v>343</v>
-      </c>
-      <c r="C110" s="21" t="s">
-        <v>344</v>
       </c>
       <c r="D110" t="s">
         <v>24</v>
@@ -5963,10 +5962,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
+        <v>344</v>
+      </c>
+      <c r="C111" s="21" t="s">
         <v>345</v>
-      </c>
-      <c r="C111" s="21" t="s">
-        <v>346</v>
       </c>
       <c r="D111" t="s">
         <v>24</v>
@@ -5995,10 +5994,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
+        <v>346</v>
+      </c>
+      <c r="C112" s="21" t="s">
         <v>347</v>
-      </c>
-      <c r="C112" s="21" t="s">
-        <v>348</v>
       </c>
       <c r="D112" t="s">
         <v>24</v>
@@ -6027,10 +6026,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
+        <v>348</v>
+      </c>
+      <c r="C113" s="21" t="s">
         <v>349</v>
-      </c>
-      <c r="C113" s="21" t="s">
-        <v>350</v>
       </c>
       <c r="D113" t="s">
         <v>24</v>
@@ -6059,10 +6058,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
+        <v>350</v>
+      </c>
+      <c r="C114" s="21" t="s">
         <v>351</v>
-      </c>
-      <c r="C114" s="21" t="s">
-        <v>352</v>
       </c>
       <c r="D114" t="s">
         <v>24</v>
@@ -6091,10 +6090,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
+        <v>352</v>
+      </c>
+      <c r="C115" s="21" t="s">
         <v>353</v>
-      </c>
-      <c r="C115" s="21" t="s">
-        <v>354</v>
       </c>
       <c r="D115" t="s">
         <v>24</v>
@@ -6123,10 +6122,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
+        <v>354</v>
+      </c>
+      <c r="C116" s="21" t="s">
         <v>355</v>
-      </c>
-      <c r="C116" s="21" t="s">
-        <v>356</v>
       </c>
       <c r="D116" t="s">
         <v>24</v>
@@ -6155,10 +6154,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
+        <v>356</v>
+      </c>
+      <c r="C117" s="21" t="s">
         <v>357</v>
-      </c>
-      <c r="C117" s="21" t="s">
-        <v>358</v>
       </c>
       <c r="D117" t="s">
         <v>24</v>
@@ -6187,10 +6186,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
+        <v>358</v>
+      </c>
+      <c r="C118" s="21" t="s">
         <v>359</v>
-      </c>
-      <c r="C118" s="21" t="s">
-        <v>360</v>
       </c>
       <c r="D118" t="s">
         <v>24</v>
@@ -6219,10 +6218,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
+        <v>360</v>
+      </c>
+      <c r="C119" s="21" t="s">
         <v>361</v>
-      </c>
-      <c r="C119" s="21" t="s">
-        <v>362</v>
       </c>
       <c r="D119" t="s">
         <v>24</v>
@@ -6251,10 +6250,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
+        <v>362</v>
+      </c>
+      <c r="C120" s="21" t="s">
         <v>363</v>
-      </c>
-      <c r="C120" s="21" t="s">
-        <v>364</v>
       </c>
       <c r="D120" t="s">
         <v>24</v>
@@ -6283,10 +6282,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
+        <v>364</v>
+      </c>
+      <c r="C121" s="21" t="s">
         <v>365</v>
-      </c>
-      <c r="C121" s="21" t="s">
-        <v>366</v>
       </c>
       <c r="D121" t="s">
         <v>24</v>
@@ -6315,10 +6314,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
+        <v>366</v>
+      </c>
+      <c r="C122" s="21" t="s">
         <v>367</v>
-      </c>
-      <c r="C122" s="21" t="s">
-        <v>368</v>
       </c>
       <c r="D122" t="s">
         <v>24</v>
@@ -6347,10 +6346,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
+        <v>368</v>
+      </c>
+      <c r="C123" s="21" t="s">
         <v>369</v>
-      </c>
-      <c r="C123" s="21" t="s">
-        <v>370</v>
       </c>
       <c r="D123" t="s">
         <v>24</v>
@@ -6379,10 +6378,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
+        <v>370</v>
+      </c>
+      <c r="C124" s="21" t="s">
         <v>371</v>
-      </c>
-      <c r="C124" s="21" t="s">
-        <v>372</v>
       </c>
       <c r="D124" t="s">
         <v>24</v>
@@ -6411,10 +6410,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
+        <v>372</v>
+      </c>
+      <c r="C125" s="21" t="s">
         <v>373</v>
-      </c>
-      <c r="C125" s="21" t="s">
-        <v>374</v>
       </c>
       <c r="D125" t="s">
         <v>24</v>
@@ -6443,10 +6442,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>374</v>
+      </c>
+      <c r="C126" s="21" t="s">
         <v>375</v>
-      </c>
-      <c r="C126" s="21" t="s">
-        <v>376</v>
       </c>
       <c r="D126" t="s">
         <v>24</v>
@@ -6475,19 +6474,19 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
+        <v>376</v>
+      </c>
+      <c r="C127" s="21" t="s">
         <v>377</v>
       </c>
-      <c r="C127" s="21" t="s">
+      <c r="D127" t="s">
+        <v>24</v>
+      </c>
+      <c r="E127" t="s">
+        <v>14</v>
+      </c>
+      <c r="F127" s="4" t="s">
         <v>378</v>
-      </c>
-      <c r="D127" t="s">
-        <v>24</v>
-      </c>
-      <c r="E127" t="s">
-        <v>14</v>
-      </c>
-      <c r="F127" s="4" t="s">
-        <v>379</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>21</v>
@@ -6504,10 +6503,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
+        <v>379</v>
+      </c>
+      <c r="C128" s="21" t="s">
         <v>380</v>
-      </c>
-      <c r="C128" s="21" t="s">
-        <v>381</v>
       </c>
       <c r="D128" t="s">
         <v>24</v>
@@ -6536,10 +6535,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
+        <v>383</v>
+      </c>
+      <c r="C129" t="s">
         <v>384</v>
-      </c>
-      <c r="C129" t="s">
-        <v>385</v>
       </c>
       <c r="D129" s="30" t="s">
         <v>13</v>
@@ -6548,16 +6547,16 @@
         <v>14</v>
       </c>
       <c r="F129" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="G129" s="4" t="s">
         <v>386</v>
-      </c>
-      <c r="G129" s="4" t="s">
-        <v>387</v>
       </c>
       <c r="H129">
         <v>1</v>
       </c>
       <c r="I129" s="29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J129" s="28" t="s">
         <v>16</v>
@@ -6580,27 +6579,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -6841,32 +6819,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBFC15CC-4CA5-447A-915F-1412CED97222}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E89B3EC5-962B-41D9-9821-3A191D2434CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{945A6BE8-5273-4FBB-A417-535A6E60D478}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6883,4 +6857,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E89B3EC5-962B-41D9-9821-3A191D2434CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBFC15CC-4CA5-447A-915F-1412CED97222}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GINI P1 (SNACKS_1703 to include direct mapping on algorithm column)
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF5B1BC-B852-45B4-AC2E-96FD6C5B0F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1106C08-0341-4B61-B7A8-7A4121247FB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="390">
   <si>
     <t>index</t>
   </si>
@@ -2023,49 +2023,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="42" builtinId="8"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2081,7 +2081,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2379,12 +2379,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H134" sqref="H134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="29" style="4" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" style="4" customWidth="1"/>
@@ -6491,6 +6491,9 @@
       <c r="G127" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="H127" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="J127" s="1" t="s">
         <v>16</v>
       </c>
@@ -6579,6 +6582,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -6819,28 +6843,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBFC15CC-4CA5-447A-915F-1412CED97222}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E89B3EC5-962B-41D9-9821-3A191D2434CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{945A6BE8-5273-4FBB-A417-535A6E60D478}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6857,29 +6885,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E89B3EC5-962B-41D9-9821-3A191D2434CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBFC15CC-4CA5-447A-915F-1412CED97222}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>